<commit_message>
Requirements and change request updated by Anvardeen Batcha B
</commit_message>
<xml_diff>
--- a/Change Request and Requirements/Change Request and Details.xlsx
+++ b/Change Request and Requirements/Change Request and Details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Change Request" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>S.No</t>
   </si>
@@ -166,13 +166,147 @@
   </si>
   <si>
     <t>While clicking course detail we need to show the details of the course.</t>
+  </si>
+  <si>
+    <t>Yete to start.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hands-on instruction.
+</t>
+  </si>
+  <si>
+    <t>Content we need to add ourself.</t>
+  </si>
+  <si>
+    <r>
+      <t>Now it's shows simply but, We need to 
+show the icon differently.  (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Only I letter icon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In course detail need to add </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Azure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> course.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Images and content we need to add ourself.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We need to modify Inet logo image.
+</t>
+  </si>
+  <si>
+    <t>While click the course under each course need to nvaigate the 
+respectived course screen.</t>
+  </si>
+  <si>
+    <r>
+      <t>Right now while click the link only it will nvaigate. But we need 
+to do for both the links. (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> See course</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Hold</t>
+  </si>
+  <si>
+    <t>Right now they want to change the inet logo alone.
+And it is in the inprogress status.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price need to hide in entire solution. </t>
+  </si>
+  <si>
+    <t>Right now price is showing as 1000 for each and every course.
+We need to hide.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +340,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -246,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -259,7 +408,10 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,18 +748,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -626,8 +777,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -636,8 +787,7 @@
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -685,6 +835,81 @@
         <v>23</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -698,7 +923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -732,7 +957,9 @@
         <v>14</v>
       </c>
       <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="D2" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -742,7 +969,9 @@
         <v>15</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
+      <c r="D3" s="6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -751,8 +980,10 @@
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -762,7 +993,9 @@
         <v>24</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>